<commit_message>
Start a Peltier drill
</commit_message>
<xml_diff>
--- a/ArrowCharts.xlsx
+++ b/ArrowCharts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{D27CAD76-2DAB-4A78-8F4A-D6A42C4761BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5759D9-9669-4EE2-BDDE-F8DB10D3773A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-564" yWindow="1008" windowWidth="14364" windowHeight="10200" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="14" r:id="rId4"/>
+    <pivotCache cacheId="15" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -359,7 +359,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -369,10 +369,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -680,69 +681,19 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Age of</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Migration</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10661027723097113"/>
+          <c:y val="0.18469696088298923"/>
+          <c:w val="0.84540805446194223"/>
+          <c:h val="0.73668486105059117"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
@@ -762,11 +713,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg2">
-                <a:lumMod val="90000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -782,13 +729,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="19050" rIns="0" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -812,6 +759,15 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -952,10 +908,8 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
+            <a:noFill/>
+            <a:ln w="12700">
               <a:noFill/>
             </a:ln>
             <a:effectLst/>
@@ -1019,6 +973,82 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="1"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Report!$E$8:$E$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="14"/>
+                  <c:pt idx="0">
+                    <c:v>0.11000000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.11</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.0000000000000008E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.06</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.13</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.0000000000000012E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>8.0000000000000016E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.03</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.0000000000000007E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>6.9999999999999993E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.05</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2.8999999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0.01</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numLit>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numLit>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="7030A0"/>
+                </a:solidFill>
+                <a:round/>
+                <a:tailEnd type="triangle" w="lg" len="lg"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>Report!$B$8:$B$21</c:f>
@@ -1163,13 +1193,18 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:effectLst>
+                  <a:glow rad="635000">
+                    <a:schemeClr val="bg1"/>
+                  </a:glow>
+                </a:effectLst>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
@@ -1182,7 +1217,7 @@
         <c:crossesAt val="-3.0000000000000006E-2"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
+        <c:lblOffset val="0"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -1256,37 +1291,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1328,6 +1332,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1880,16 +1885,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1914,10 +1919,163 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>549966</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>145774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>86140</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>159026</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8D33941-5C74-9835-E3C0-D1D38E56F6E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5380383" y="974035"/>
+          <a:ext cx="2584174" cy="344556"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" tIns="0" bIns="0" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000"/>
+            <a:t>Share</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" baseline="0"/>
+            <a:t> of population that was foreign born in 1990 and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="1" baseline="0"/>
+            <a:t>2020</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.1019</cdr:x>
+      <cdr:y>0.00727</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.56386</cdr:x>
+      <cdr:y>0.07273</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA15178A-6486-49C7-9946-85D9CC28B548}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="496957" y="26504"/>
+          <a:ext cx="2252869" cy="238539"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Age of Migration</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2209,7 +2367,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -2503,8 +2661,8 @@
   </sheetPr>
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2536,7 +2694,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>45455</v>
       </c>
       <c r="C3" s="2"/>
@@ -2556,13 +2714,13 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="9">
         <v>0.09</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>0.2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <f>D8-C8</f>
         <v>0.11000000000000001</v>
       </c>
@@ -2571,13 +2729,13 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9">
         <v>0.08</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="9">
         <v>0.19</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <f t="shared" ref="E9:E21" si="0">D9-C9</f>
         <v>0.11</v>
       </c>
@@ -2586,13 +2744,13 @@
       <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>0.13</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="9">
         <v>0.17</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <f t="shared" si="0"/>
         <v>4.0000000000000008E-2</v>
       </c>
@@ -2601,13 +2759,13 @@
       <c r="B11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="9">
         <v>0.09</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="9">
         <v>0.15</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
@@ -2616,13 +2774,13 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <v>0.02</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="9">
         <v>0.15</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <f t="shared" si="0"/>
         <v>0.13</v>
       </c>
@@ -2631,13 +2789,13 @@
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="10">
+      <c r="C13" s="9">
         <v>0.08</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="9">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <f t="shared" si="0"/>
         <v>6.0000000000000012E-2</v>
       </c>
@@ -2646,13 +2804,13 @@
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>0.06</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="9">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="9">
         <f t="shared" si="0"/>
         <v>8.0000000000000016E-2</v>
       </c>
@@ -2661,13 +2819,13 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="9">
         <v>0.1</v>
       </c>
-      <c r="D15" s="10">
+      <c r="D15" s="9">
         <v>0.13</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="9">
         <f t="shared" si="0"/>
         <v>0.03</v>
       </c>
@@ -2676,13 +2834,13 @@
       <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>0.06</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>0.13</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="9">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
@@ -2691,13 +2849,13 @@
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="9">
         <v>0.05</v>
       </c>
-      <c r="D17" s="10">
+      <c r="D17" s="9">
         <v>0.12</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="9">
         <f t="shared" si="0"/>
         <v>6.9999999999999993E-2</v>
       </c>
@@ -2706,13 +2864,13 @@
       <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="9">
         <v>0.03</v>
       </c>
-      <c r="D18" s="10">
+      <c r="D18" s="9">
         <v>0.11</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="9">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
@@ -2721,13 +2879,13 @@
       <c r="B19" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <v>0.02</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="9">
         <f t="shared" si="0"/>
         <v>0.05</v>
       </c>
@@ -2736,13 +2894,13 @@
       <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="11">
+      <c r="C20" s="10">
         <v>1E-3</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>0.03</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <f t="shared" si="0"/>
         <v>2.8999999999999998E-2</v>
       </c>
@@ -2751,13 +2909,13 @@
       <c r="B21" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>0.01</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>0.02</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
@@ -2943,19 +3101,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -2963,11 +3117,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -2975,19 +3128,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -2995,11 +3144,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -3007,19 +3155,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -3027,11 +3171,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -3039,13 +3182,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Starting to add another arrow chart example
</commit_message>
<xml_diff>
--- a/ArrowCharts.xlsx
+++ b/ArrowCharts.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5759D9-9669-4EE2-BDDE-F8DB10D3773A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCE9977-17DA-42B4-941B-F560A77B5C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-53760" yWindow="1110" windowWidth="28890" windowHeight="15915" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report" sheetId="1" r:id="rId1"/>
+    <sheet name="MigrationChart" sheetId="1" r:id="rId1"/>
     <sheet name="Formats" sheetId="2" r:id="rId2"/>
     <sheet name="Lists" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>FROM:</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>Italy</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -359,7 +362,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -374,6 +377,7 @@
     <xf numFmtId="15" fontId="6" fillId="4" borderId="0" xfId="8" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="12"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -703,7 +707,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Report!$D$7</c:f>
+              <c:f>MigrationChart!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -763,10 +767,6 @@
                   <a:prstGeom prst="rect">
                     <a:avLst/>
                   </a:prstGeom>
-                  <a:noFill/>
-                  <a:ln>
-                    <a:noFill/>
-                  </a:ln>
                 </c15:spPr>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -788,7 +788,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Report!$B$8:$B$21</c:f>
+              <c:f>MigrationChart!$B$8:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -838,7 +838,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Report!$D$8:$D$21</c:f>
+              <c:f>MigrationChart!$D$8:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="14"/>
@@ -898,7 +898,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Report!$C$7</c:f>
+              <c:f>MigrationChart!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -979,7 +979,7 @@
             <c:noEndCap val="1"/>
             <c:plus>
               <c:numRef>
-                <c:f>Report!$E$8:$E$21</c:f>
+                <c:f>MigrationChart!$E$8:$E$21</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="14"/>
@@ -1051,7 +1051,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Report!$B$8:$B$21</c:f>
+              <c:f>MigrationChart!$B$8:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
@@ -1101,7 +1101,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Report!$C$8:$C$21</c:f>
+              <c:f>MigrationChart!$C$8:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1332,553 +1332,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1922,15 +1376,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>549966</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>145774</xdr:rowOff>
+      <xdr:colOff>276640</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>119767</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>86140</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>431442</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>159026</xdr:rowOff>
+      <xdr:rowOff>146271</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1945,8 +1399,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5380383" y="974035"/>
-          <a:ext cx="2584174" cy="344556"/>
+          <a:off x="5113683" y="815506"/>
+          <a:ext cx="2606455" cy="548308"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1955,11 +1409,7 @@
           <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
+          <a:noFill/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1979,6 +1429,12 @@
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" tIns="0" bIns="0" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1"/>
+            <a:t>Age of Migration </a:t>
+          </a:r>
+        </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1000"/>
@@ -2002,80 +1458,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.1019</cdr:x>
-      <cdr:y>0.00727</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.56386</cdr:x>
-      <cdr:y>0.07273</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA15178A-6486-49C7-9946-85D9CC28B548}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="496957" y="26504"/>
-          <a:ext cx="2252869" cy="238539"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-            <a:lnSpc>
-              <a:spcPct val="100000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPts val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPts val="0"/>
-            </a:spcAft>
-            <a:buClrTx/>
-            <a:buSzTx/>
-            <a:buFontTx/>
-            <a:buNone/>
-            <a:tabLst/>
-            <a:defRPr/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" i="0" baseline="0">
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Age of Migration</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2147,8 +1529,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3166111" y="270455"/>
-          <a:ext cx="2200275" cy="491546"/>
+          <a:off x="3158491" y="270455"/>
+          <a:ext cx="2205990" cy="510596"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="502976"/>
         </a:xfrm>
@@ -2659,10 +2041,10 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2672,7 +2054,7 @@
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2681,7 +2063,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2689,8 +2071,11 @@
         <v>32</v>
       </c>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2699,7 +2084,7 @@
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>1990</v>
       </c>
@@ -2710,7 +2095,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>21</v>
       </c>
@@ -2725,7 +2110,7 @@
         <v>0.11000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>22</v>
       </c>
@@ -2740,7 +2125,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -2755,7 +2140,7 @@
         <v>4.0000000000000008E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -2770,7 +2155,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -2785,7 +2170,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>26</v>
       </c>
@@ -2800,7 +2185,7 @@
         <v>6.0000000000000012E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -2815,7 +2200,7 @@
         <v>8.0000000000000016E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>28</v>
       </c>
@@ -2830,7 +2215,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>29</v>
       </c>
@@ -2921,9 +2306,12 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" location="respond" xr:uid="{801373B0-9ED9-4824-A7D7-E2926FFD0D4F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -2965,7 +2353,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>12-Jun-2024</v>
+        <v>13-Jun-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3261,7 +2649,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>12-Jun-2024</v>
+        <v>13-Jun-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Two way arrow charts
</commit_message>
<xml_diff>
--- a/ArrowCharts.xlsx
+++ b/ArrowCharts.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCE9977-17DA-42B4-941B-F560A77B5C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77603BF9-DA98-49B1-9761-2BD33F53BA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53760" yWindow="1110" windowWidth="28890" windowHeight="15915" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-28950" yWindow="-2730" windowWidth="28890" windowHeight="15915" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="MigrationChart" sheetId="1" r:id="rId1"/>
-    <sheet name="Formats" sheetId="2" r:id="rId2"/>
-    <sheet name="Lists" sheetId="3" r:id="rId3"/>
+    <sheet name="AnotherArrowChartExample" sheetId="4" r:id="rId2"/>
+    <sheet name="Formats" sheetId="2" r:id="rId3"/>
+    <sheet name="Lists" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId4"/>
+    <pivotCache cacheId="16" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>FROM:</t>
   </si>
@@ -178,6 +179,42 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Gain</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Albany</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>Canton</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>El Paso</t>
+  </si>
+  <si>
+    <t>Fresno</t>
   </si>
 </sst>
 </file>
@@ -653,9 +690,10 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF4747"/>
+      <color rgb="FFFF9999"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFEBFFEB"/>
-      <color rgb="FFFF9999"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FFEFFFEF"/>
     </mruColors>
@@ -1335,6 +1373,1082 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Arrow Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.7805938320209979E-2"/>
+          <c:y val="3.7037037037037035E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AnotherArrowChartExample!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>AnotherArrowChartExample!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Albany</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Boston</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Canton</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Denver</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>El Paso</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fresno</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnotherArrowChartExample!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.71</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BFB7-44DB-B8DF-6BAE71D27A52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AnotherArrowChartExample!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gain</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="1"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="0070C0"/>
+                </a:solidFill>
+                <a:round/>
+                <a:headEnd type="stealth" w="lg" len="med"/>
+                <a:tailEnd type="oval"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>AnotherArrowChartExample!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Albany</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Boston</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Canton</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Denver</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>El Paso</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fresno</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnotherArrowChartExample!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.58999999999999986</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.49999999999999978</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BFB7-44DB-B8DF-6BAE71D27A52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>AnotherArrowChartExample!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Loss</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:noEndCap val="1"/>
+            <c:val val="100"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:srgbClr val="FF4747"/>
+                </a:solidFill>
+                <a:round/>
+                <a:headEnd type="oval" w="med" len="med"/>
+                <a:tailEnd type="stealth" w="lg" len="med"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>AnotherArrowChartExample!$B$3:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Albany</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Boston</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Canton</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Denver</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>El Paso</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Fresno</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AnotherArrowChartExample!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>#N/A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.37999999999999989</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BFB7-44DB-B8DF-6BAE71D27A52}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="946802704"/>
+        <c:axId val="946803184"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="946802704"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="946803184"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="946803184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="946802704"/>
+        <c:crosses val="max"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1458,6 +2572,216 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>605790</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>382905</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>56</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4EE56E-4ED3-4A70-A1F3-9FBC49CB5A00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4711065" y="0"/>
+          <a:ext cx="2215515" cy="523931"/>
+          <a:chOff x="3162301" y="274265"/>
+          <a:chExt cx="2198370" cy="502976"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="3" name="TextBox 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9DC1B88-9EF0-C10B-0955-4DD876B33B84}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3162301" y="274265"/>
+            <a:ext cx="715113" cy="502976"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>FROM:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>SUBJECT:</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="1"/>
+              <a:t>DATE:</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="TextBox 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BED8DE4-FE55-77B2-4CDF-89E8E26EC17D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3876370" y="274265"/>
+            <a:ext cx="1484301" cy="502976"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>Mark Biegert</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>Another Arrow</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0" baseline="0"/>
+              <a:t> Chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" sz="1100" b="0"/>
+              <a:t>13-June-2024</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{244A75F4-8231-D639-7284-FA68B2C23648}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1749,7 +3073,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -2043,7 +3367,7 @@
   </sheetPr>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
@@ -2316,6 +3640,195 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE13FC8-6F1E-4DBF-9704-C5023FF32D19}">
+  <dimension ref="A1:L8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="10" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>3.66</v>
+      </c>
+      <c r="D3">
+        <v>4.25</v>
+      </c>
+      <c r="E3">
+        <f>MIN(C3:D3)</f>
+        <v>3.66</v>
+      </c>
+      <c r="F3">
+        <f>IF(D3&gt;C3,D3-C3,NA())</f>
+        <v>0.58999999999999986</v>
+      </c>
+      <c r="G3" t="e">
+        <f>IF(C3&gt;D3,C3-D3,NA())</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>3.21</v>
+      </c>
+      <c r="D4">
+        <v>2.65</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E8" si="0">MIN(C4:D4)</f>
+        <v>2.65</v>
+      </c>
+      <c r="F4" t="e">
+        <f t="shared" ref="F4:F8" si="1">IF(D4&gt;C4,D4-C4,NA())</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G8" si="2">IF(C4&gt;D4,C4-D4,NA())</f>
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5">
+        <v>2.57</v>
+      </c>
+      <c r="D5">
+        <v>3.11</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>2.57</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>0.54</v>
+      </c>
+      <c r="G5" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>2.15</v>
+      </c>
+      <c r="D6">
+        <v>1.71</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1.71</v>
+      </c>
+      <c r="F6" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>0.43999999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7">
+        <v>1.59</v>
+      </c>
+      <c r="D7">
+        <v>2.09</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>1.59</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>0.49999999999999978</v>
+      </c>
+      <c r="G7" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8">
+        <v>1.41</v>
+      </c>
+      <c r="D8">
+        <v>1.03</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>1.03</v>
+      </c>
+      <c r="F8" t="e">
+        <f t="shared" si="1"/>
+        <v>#N/A</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>0.37999999999999989</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L7" r:id="rId1" xr:uid="{0826D535-8E8A-4B8C-9E40-612E3D735B57}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912E8867-A2D1-43A4-9ACC-7AB2760F7CD8}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -2323,7 +3836,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2614,7 +4127,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E13436D-CE0C-4639-B951-C1B98556791F}">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>

</xml_diff>